<commit_message>
reruns with updated data 29 July
</commit_message>
<xml_diff>
--- a/02_sampleclip.xlsx
+++ b/02_sampleclip.xlsx
@@ -42515,7 +42515,7 @@
       </c>
       <c r="G89" t="inlineStr"/>
       <c r="H89" t="n">
-        <v>0.5465465465465461</v>
+        <v>0.5454545454545454</v>
       </c>
       <c r="I89" t="n">
         <v>0.2252817716958035</v>
@@ -42989,7 +42989,7 @@
         </is>
       </c>
       <c r="H103" t="n">
-        <v>0.5465465465465468</v>
+        <v>0.5454545454545454</v>
       </c>
       <c r="I103" t="n">
         <v>0.2040116928782406</v>
@@ -43253,7 +43253,7 @@
       </c>
       <c r="G111" t="inlineStr"/>
       <c r="H111" t="n">
-        <v>0.1165048543689313</v>
+        <v>0.1176470588235294</v>
       </c>
       <c r="I111" t="n">
         <v>0.2037073644682586</v>
@@ -43517,7 +43517,7 @@
         </is>
       </c>
       <c r="H119" t="n">
-        <v>0.4175824175824164</v>
+        <v>0.4166666666666667</v>
       </c>
       <c r="I119" t="n">
         <v>0.2242150469444044</v>
@@ -43929,7 +43929,7 @@
         </is>
       </c>
       <c r="H131" t="n">
-        <v>0.4534534534534526</v>
+        <v>0.4545454545454545</v>
       </c>
       <c r="I131" t="n">
         <v>0.2211791160666618</v>
@@ -44644,7 +44644,7 @@
         </is>
       </c>
       <c r="H152" t="n">
-        <v>0.1766990291262141</v>
+        <v>0.1764705882352941</v>
       </c>
       <c r="I152" t="n">
         <v>0.2010269041579556</v>
@@ -45169,7 +45169,7 @@
         </is>
       </c>
       <c r="H167" t="n">
-        <v>0.2847058823529403</v>
+        <v>0.2857142857142857</v>
       </c>
       <c r="I167" t="n">
         <v>0.2268614230960211</v>
@@ -45593,10 +45593,10 @@
         </is>
       </c>
       <c r="H179" t="n">
-        <v>0.309644670050761</v>
+        <v>0.25</v>
       </c>
       <c r="I179" t="n">
-        <v>0.2351637737132817</v>
+        <v>0.235552401210024</v>
       </c>
       <c r="J179" t="inlineStr"/>
       <c r="K179" t="inlineStr"/>
@@ -45736,12 +45736,8 @@
           <t>L4</t>
         </is>
       </c>
-      <c r="H183" t="n">
-        <v>0.2141176470588241</v>
-      </c>
-      <c r="I183" t="n">
-        <v>0.2379054448708635</v>
-      </c>
+      <c r="H183" t="inlineStr"/>
+      <c r="I183" t="inlineStr"/>
       <c r="J183" t="inlineStr"/>
       <c r="K183" t="inlineStr"/>
     </row>
@@ -45774,7 +45770,7 @@
       <c r="H184" t="inlineStr"/>
       <c r="I184" t="inlineStr"/>
       <c r="J184" t="n">
-        <v>0.1257731958762885</v>
+        <v>0.125</v>
       </c>
       <c r="K184" t="n">
         <v>0.2383047117077986</v>
@@ -45838,7 +45834,7 @@
       </c>
       <c r="G186" t="inlineStr"/>
       <c r="H186" t="n">
-        <v>0.5840220385674917</v>
+        <v>0.5833333333333334</v>
       </c>
       <c r="I186" t="n">
         <v>0.2413428386587952</v>
@@ -46153,10 +46149,10 @@
         </is>
       </c>
       <c r="H195" t="n">
-        <v>0.8901098901098923</v>
+        <v>0.5625</v>
       </c>
       <c r="I195" t="n">
-        <v>0.2409480558409915</v>
+        <v>0.2406595647040624</v>
       </c>
       <c r="J195" t="inlineStr"/>
       <c r="K195" t="inlineStr"/>
@@ -46432,12 +46428,8 @@
           <t>L4</t>
         </is>
       </c>
-      <c r="H203" t="n">
-        <v>0.06185567010309143</v>
-      </c>
-      <c r="I203" t="n">
-        <v>0.2383516356086297</v>
-      </c>
+      <c r="H203" t="inlineStr"/>
+      <c r="I203" t="inlineStr"/>
       <c r="J203" t="inlineStr"/>
       <c r="K203" t="inlineStr"/>
     </row>
@@ -46682,10 +46674,10 @@
         </is>
       </c>
       <c r="H210" t="n">
-        <v>0.0660792951541856</v>
+        <v>0.3461538461538461</v>
       </c>
       <c r="I210" t="n">
-        <v>0.2336534371307401</v>
+        <v>0.2302721350178679</v>
       </c>
       <c r="J210" t="inlineStr"/>
       <c r="K210" t="inlineStr"/>
@@ -46720,12 +46712,8 @@
           <t>L4</t>
         </is>
       </c>
-      <c r="H211" t="n">
-        <v>0.7765567765567765</v>
-      </c>
-      <c r="I211" t="n">
-        <v>0.2304253284954803</v>
-      </c>
+      <c r="H211" t="inlineStr"/>
+      <c r="I211" t="inlineStr"/>
       <c r="J211" t="inlineStr"/>
       <c r="K211" t="inlineStr"/>
     </row>
@@ -46969,12 +46957,8 @@
           <t>R4</t>
         </is>
       </c>
-      <c r="H218" t="n">
-        <v>0.05677655677655628</v>
-      </c>
-      <c r="I218" t="n">
-        <v>0.2258184785617093</v>
-      </c>
+      <c r="H218" t="inlineStr"/>
+      <c r="I218" t="inlineStr"/>
       <c r="J218" t="inlineStr"/>
       <c r="K218" t="inlineStr"/>
     </row>
@@ -47316,7 +47300,7 @@
       </c>
       <c r="G228" t="inlineStr"/>
       <c r="H228" t="n">
-        <v>0.060194174757281</v>
+        <v>0.05882352941176471</v>
       </c>
       <c r="I228" t="n">
         <v>0.2097981067699299</v>
@@ -47421,10 +47405,10 @@
         </is>
       </c>
       <c r="H231" t="n">
-        <v>0.3622754491017955</v>
+        <v>0.1818181818181818</v>
       </c>
       <c r="I231" t="n">
-        <v>0.201614405373553</v>
+        <v>0.2038203830775984</v>
       </c>
       <c r="J231" t="inlineStr"/>
       <c r="K231" t="inlineStr"/>
@@ -47497,7 +47481,7 @@
       <c r="H233" t="inlineStr"/>
       <c r="I233" t="inlineStr"/>
       <c r="J233" t="n">
-        <v>0.1522842639593898</v>
+        <v>0.1538461538461539</v>
       </c>
       <c r="K233" t="n">
         <v>0.1994084276695075</v>
@@ -47569,7 +47553,7 @@
         </is>
       </c>
       <c r="H235" t="n">
-        <v>0.4026402640264024</v>
+        <v>0.4</v>
       </c>
       <c r="I235" t="n">
         <v>0.1913971773640999</v>
@@ -47969,10 +47953,10 @@
         </is>
       </c>
       <c r="H247" t="n">
-        <v>0.8019801980198032</v>
+        <v>0.6</v>
       </c>
       <c r="I247" t="n">
-        <v>0.1414253795812333</v>
+        <v>0.1467493551492729</v>
       </c>
       <c r="J247" t="inlineStr"/>
       <c r="K247" t="inlineStr"/>
@@ -48185,10 +48169,10 @@
       <c r="H253" t="inlineStr"/>
       <c r="I253" t="inlineStr"/>
       <c r="J253" t="n">
-        <v>0.1257731958762887</v>
+        <v>0.125</v>
       </c>
       <c r="K253" t="n">
-        <v>0.1307774284451542</v>
+        <v>0.1320374501534733</v>
       </c>
     </row>
     <row r="254">
@@ -48257,7 +48241,7 @@
         </is>
       </c>
       <c r="H255" t="n">
-        <v>0.06593406593406648</v>
+        <v>0.06666666666666667</v>
       </c>
       <c r="I255" t="n">
         <v>0.1282573850285159</v>
@@ -48742,7 +48726,7 @@
         </is>
       </c>
       <c r="H270" t="n">
-        <v>0.05825242718446472</v>
+        <v>0.05882352941176471</v>
       </c>
       <c r="I270" t="n">
         <v>0.1783621648177678</v>
@@ -48956,7 +48940,7 @@
         </is>
       </c>
       <c r="H276" t="n">
-        <v>0.3071065989847726</v>
+        <v>0.3076923076923077</v>
       </c>
       <c r="I276" t="n">
         <v>0.2154716513900335</v>
@@ -49399,7 +49383,7 @@
         </is>
       </c>
       <c r="H289" t="n">
-        <v>0.3071065989847726</v>
+        <v>0.3076923076923077</v>
       </c>
       <c r="I289" t="n">
         <v>0.2238686101387339</v>
@@ -49648,10 +49632,10 @@
         </is>
       </c>
       <c r="H296" t="n">
-        <v>0.1184466019417473</v>
+        <v>0.05882352941176471</v>
       </c>
       <c r="I296" t="n">
-        <v>0.2182927912051581</v>
+        <v>0.2191224641961304</v>
       </c>
       <c r="J296" t="inlineStr"/>
       <c r="K296" t="inlineStr"/>
@@ -50130,10 +50114,10 @@
         </is>
       </c>
       <c r="H310" t="n">
-        <v>0.455089820359285</v>
+        <v>0.2727272727272727</v>
       </c>
       <c r="I310" t="n">
-        <v>0.197699561374115</v>
+        <v>0.1973309052259164</v>
       </c>
       <c r="J310" t="inlineStr"/>
       <c r="K310" t="inlineStr"/>
@@ -50421,10 +50405,10 @@
         </is>
       </c>
       <c r="H319" t="n">
-        <v>0.1340659340659339</v>
+        <v>0.1333333333333333</v>
       </c>
       <c r="I319" t="n">
-        <v>0.2154172730240809</v>
+        <v>0.2137491315702116</v>
       </c>
       <c r="J319" t="inlineStr"/>
       <c r="K319" t="inlineStr"/>
@@ -50670,7 +50654,7 @@
         </is>
       </c>
       <c r="H326" t="n">
-        <v>0.1548223350253805</v>
+        <v>0.1538461538461539</v>
       </c>
       <c r="I326" t="n">
         <v>0.2344804239811755</v>
@@ -51222,10 +51206,10 @@
         </is>
       </c>
       <c r="H342" t="n">
-        <v>0.7765567765567765</v>
+        <v>0.2222222222222222</v>
       </c>
       <c r="I342" t="n">
-        <v>0.2115506342458336</v>
+        <v>0.2186247114504461</v>
       </c>
       <c r="J342" t="inlineStr"/>
       <c r="K342" t="inlineStr"/>
@@ -51533,7 +51517,7 @@
       </c>
       <c r="G351" t="inlineStr"/>
       <c r="H351" t="n">
-        <v>0.1162790697674428</v>
+        <v>0.1176470588235294</v>
       </c>
       <c r="I351" t="n">
         <v>0.1980035978381223</v>
@@ -51770,7 +51754,7 @@
         </is>
       </c>
       <c r="H358" t="n">
-        <v>0.2004405286343633</v>
+        <v>0.2</v>
       </c>
       <c r="I358" t="n">
         <v>0.2020126393680249</v>
@@ -52264,7 +52248,7 @@
         </is>
       </c>
       <c r="H372" t="n">
-        <v>0.05825242718446472</v>
+        <v>0.05882352941176471</v>
       </c>
       <c r="I372" t="n">
         <v>0.2356152236473341</v>
@@ -52540,7 +52524,7 @@
         </is>
       </c>
       <c r="H380" t="n">
-        <v>0.5449101796407203</v>
+        <v>0.5454545454545454</v>
       </c>
       <c r="I380" t="n">
         <v>0.2561965785613409</v>
@@ -52925,7 +52909,7 @@
         </is>
       </c>
       <c r="H391" t="n">
-        <v>0.2853773584905662</v>
+        <v>0.3076923076923077</v>
       </c>
       <c r="I391" t="n">
         <v>0.2540834818368891</v>
@@ -53768,7 +53752,7 @@
       </c>
       <c r="G416" t="inlineStr"/>
       <c r="H416" t="n">
-        <v>0.08539944903581438</v>
+        <v>0.09090909090909091</v>
       </c>
       <c r="I416" t="n">
         <v>0.1724637162897068</v>
@@ -54129,7 +54113,7 @@
         </is>
       </c>
       <c r="H427" t="n">
-        <v>0.4986225895316788</v>
+        <v>0.5</v>
       </c>
       <c r="I427" t="n">
         <v>0.174012687922756</v>
@@ -55450,7 +55434,7 @@
         </is>
       </c>
       <c r="H466" t="n">
-        <v>0.6006600660066038</v>
+        <v>0.6</v>
       </c>
       <c r="I466" t="n">
         <v>0.1723071642810401</v>
@@ -55967,7 +55951,7 @@
       </c>
       <c r="G481" t="inlineStr"/>
       <c r="H481" t="n">
-        <v>0.1876288659793795</v>
+        <v>0.1875</v>
       </c>
       <c r="I481" t="n">
         <v>0.2168901172670945</v>
@@ -56593,7 +56577,7 @@
         </is>
       </c>
       <c r="H499" t="n">
-        <v>0.3760330578512382</v>
+        <v>0.3333333333333333</v>
       </c>
       <c r="I499" t="n">
         <v>0.0948207702818341</v>

</xml_diff>